<commit_message>
Updated sync helper to work with new format of files. Sorting before creating json to help in comparing. Other fixes
</commit_message>
<xml_diff>
--- a/tools/mayan_sync_helper/xml_definitions/doctype_definitions.xlsx
+++ b/tools/mayan_sync_helper/xml_definitions/doctype_definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\pims\PSP\tools\mayan_sync_helper\xml_definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141F3229-BEBC-4E92-8A7B-606714F367F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D69F2FF-584D-4B3D-9DB4-77D2E8D16463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22320" yWindow="240" windowWidth="22185" windowHeight="20505" xr2:uid="{B36D4D41-52C3-4254-819B-044EB561F7B6}"/>
+    <workbookView xWindow="-38265" yWindow="0" windowWidth="18750" windowHeight="20985" xr2:uid="{B36D4D41-52C3-4254-819B-044EB561F7B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="195">
   <si>
     <t>Document type</t>
   </si>
@@ -427,175 +427,202 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>testing purpose 1</t>
-  </si>
-  <si>
-    <t>testing purpose 2</t>
-  </si>
-  <si>
-    <t>testing purpose 3</t>
-  </si>
-  <si>
-    <t>testing purpose 4</t>
-  </si>
-  <si>
-    <t>testing purpose 5</t>
-  </si>
-  <si>
-    <t>testing purpose 6</t>
-  </si>
-  <si>
-    <t>testing purpose 7</t>
-  </si>
-  <si>
-    <t>testing purpose 8</t>
-  </si>
-  <si>
-    <t>testing purpose 9</t>
-  </si>
-  <si>
-    <t>testing purpose 10</t>
-  </si>
-  <si>
-    <t>testing purpose 11</t>
-  </si>
-  <si>
-    <t>testing purpose 12</t>
-  </si>
-  <si>
-    <t>testing purpose 13</t>
-  </si>
-  <si>
-    <t>testing purpose 14</t>
-  </si>
-  <si>
-    <t>testing purpose 15</t>
-  </si>
-  <si>
-    <t>testing purpose 16</t>
-  </si>
-  <si>
-    <t>testing purpose 17</t>
-  </si>
-  <si>
-    <t>testing purpose 18</t>
-  </si>
-  <si>
-    <t>testing purpose 19</t>
-  </si>
-  <si>
-    <t>testing purpose 20</t>
-  </si>
-  <si>
-    <t>testing purpose 21</t>
-  </si>
-  <si>
-    <t>testing purpose 22</t>
-  </si>
-  <si>
-    <t>testing purpose 23</t>
-  </si>
-  <si>
-    <t>testing purpose 24</t>
-  </si>
-  <si>
-    <t>testing purpose 25</t>
-  </si>
-  <si>
-    <t>testing purpose 26</t>
-  </si>
-  <si>
-    <t>testing purpose 27</t>
-  </si>
-  <si>
-    <t>testing purpose 28</t>
-  </si>
-  <si>
-    <t>testing purpose 29</t>
-  </si>
-  <si>
-    <t>testing purpose 30</t>
-  </si>
-  <si>
-    <t>testing purpose 31</t>
-  </si>
-  <si>
-    <t>testing purpose 32</t>
-  </si>
-  <si>
-    <t>testing purpose 33</t>
-  </si>
-  <si>
-    <t>testing purpose 34</t>
-  </si>
-  <si>
-    <t>testing purpose 35</t>
-  </si>
-  <si>
-    <t>testing purpose 36</t>
-  </si>
-  <si>
-    <t>testing purpose 37</t>
-  </si>
-  <si>
-    <t>testing purpose 38</t>
-  </si>
-  <si>
-    <t>testing purpose 39</t>
-  </si>
-  <si>
-    <t>testing purpose 40</t>
-  </si>
-  <si>
-    <t>testing purpose 41</t>
-  </si>
-  <si>
-    <t>testing purpose 42</t>
-  </si>
-  <si>
-    <t>testing purpose 43</t>
-  </si>
-  <si>
-    <t>testing purpose 44</t>
-  </si>
-  <si>
-    <t>testing purpose 45</t>
-  </si>
-  <si>
-    <t>testing purpose 46</t>
-  </si>
-  <si>
-    <t>testing purpose 47</t>
-  </si>
-  <si>
-    <t>testing purpose 48</t>
-  </si>
-  <si>
-    <t>testing purpose 49</t>
-  </si>
-  <si>
-    <t>testing purpose 50</t>
-  </si>
-  <si>
-    <t>testing purpose 51</t>
-  </si>
-  <si>
-    <t>testing purpose 52</t>
-  </si>
-  <si>
-    <t>testing purpose 53</t>
-  </si>
-  <si>
-    <t>testing purpose 54</t>
-  </si>
-  <si>
-    <t>testing purpose 55</t>
-  </si>
-  <si>
-    <t>testing purpose 56</t>
-  </si>
-  <si>
-    <t>testing purpose 57</t>
+    <t xml:space="preserve">The Affidavit of Services and correspondence with the Process Server </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For ALC Applications, Orders, and Resolutions </t>
+  </si>
+  <si>
+    <t>Form 5 - Approval of expropriation</t>
+  </si>
+  <si>
+    <t>The Approval of Expropriation (Form 5) for Expropriations</t>
+  </si>
+  <si>
+    <t>Appraisals property in draft / final state</t>
+  </si>
+  <si>
+    <t>BC Assessment search</t>
+  </si>
+  <si>
+    <t>Draft / final versions of the briefing notes</t>
+  </si>
+  <si>
+    <t>Surveys registered in the Canada Land System.</t>
+  </si>
+  <si>
+    <t>Templates used for document generation in PIMS</t>
+  </si>
+  <si>
+    <t>The Certificate of Compliance (CoC)</t>
+  </si>
+  <si>
+    <t>The Certificate of Insurance H.0111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The compensation cheque </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The H.120 Compensation Requisitions </t>
+  </si>
+  <si>
+    <t>The company search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H.0443 Conditions of Entry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The conveyance closing documents which might include PTT, Form A Transfer, or Statement of Adjustments. </t>
+  </si>
+  <si>
+    <t>Attach letters, memos, emails (not record of negotiation, or legal correspondence)</t>
+  </si>
+  <si>
+    <t>The crown grant application and final crown grant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The District road register </t>
+  </si>
+  <si>
+    <t>The Referral Record for both incoming and outgoing referrals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The survey field notes </t>
+  </si>
+  <si>
+    <t>Financial records (invoices, journal vouchers, received cheques etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial records which could include invoices, JV’s, contracts ect. </t>
+  </si>
+  <si>
+    <t>Record of engagement with first nations (ex: First Nations Consultation Log)</t>
+  </si>
+  <si>
+    <t>The First Nation Strength of Claim report</t>
+  </si>
+  <si>
+    <t>Form 12 - Certificate As To Highway In Statutory Right Of Way Plan, pre and post registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gazette notices – all types of gazettes (establishing, closing, widening, erratum’s) </t>
+  </si>
+  <si>
+    <t>All types of scanned documents from a historical file</t>
+  </si>
+  <si>
+    <t>Applications and final Land Act Tenure Reserves (Sections 15/16/17)</t>
+  </si>
+  <si>
+    <t>Lease / License agreement</t>
+  </si>
+  <si>
+    <t>Draft or Final Lease/License agreement, amending agreement or extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emails or letters with internal and external lawyers </t>
+  </si>
+  <si>
+    <t>Attach copies of legal survey plans, draft or registered versions</t>
+  </si>
+  <si>
+    <t>Approval/sign-off</t>
+  </si>
+  <si>
+    <t>The record of correspondence (email) approving Lease/Licence</t>
+  </si>
+  <si>
+    <t>Attach LTSA documents ie: copies of mortgages, SRW’s, Easements, Pending Litigation (except title searches and legal plans)</t>
+  </si>
+  <si>
+    <t>Ministerial Orders</t>
+  </si>
+  <si>
+    <t>Miscellaneous Notes from the property title</t>
+  </si>
+  <si>
+    <t>Moti Plans, plans not found in LTSA (Road Surveys)</t>
+  </si>
+  <si>
+    <t>NOTIABANDON</t>
+  </si>
+  <si>
+    <t>Form 7 - Notice of abandonement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form 8 - Notice of advanced payment </t>
+  </si>
+  <si>
+    <t>The Notice of Advance Payment  (Form 8) for Expropriation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Notice of Claims/Litigation documents </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form 1 - Notice of expropriation </t>
+  </si>
+  <si>
+    <t>The Notice of Expropriation (Form 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Notice of Possible Entry (H.0224) </t>
+  </si>
+  <si>
+    <t>The Order in Council</t>
+  </si>
+  <si>
+    <t>Uncategorized / Miscellaneous document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other forms of Land Agreements such as Indemnity Letters, Letter of Intended Use, Assumption Agreements etc. </t>
+  </si>
+  <si>
+    <t>Attach copies of draft or final Offer to Purchase agreements (H.179s) or external Owner agreements for Offer and Purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property acquisition drawings, design drawings, engineered drawings in draft and final versions </t>
+  </si>
+  <si>
+    <t>Attach Photos, images or videos relevant to file/property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Privy Council </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional/Expert Report in draft or final (Ie: Geotechnical, Environmental, Archeology, Engineering Reports)  </t>
+  </si>
+  <si>
+    <t>The Purchase and Sale Agreement for a road closure file (H.179RC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Record of Negotiations </t>
+  </si>
+  <si>
+    <t>The Release of Claims document, Draft and Final versions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Spending Authority Approval (SAA) document, Draft and Final versions </t>
+  </si>
+  <si>
+    <t>The Surplus Property Declarations document in Draft or Final indicating surplus land</t>
+  </si>
+  <si>
+    <t>Tax notices or Tax assessments</t>
+  </si>
+  <si>
+    <t>The Temporary License for Construction Access Agreement (TLCA) Draft or Final version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Title Search from LTSA which could be a current or historical search </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Transfer of Administration (TAC) document – Draft or Final version </t>
+  </si>
+  <si>
+    <t>Form 9 - Vesting notice (Form 9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Vesting Notice (Form 9) for Expropriations </t>
   </si>
 </sst>
 </file>
@@ -604,14 +631,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -638,9 +657,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FFB6C2CF"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -664,7 +690,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -687,31 +713,425 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -722,6 +1142,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90B7AD45-2D83-4071-903A-709897297D7D}" name="Table1" displayName="Table1" ref="B2:J60" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="11" totalsRowBorderDxfId="10" headerRowCellStyle="Normal">
+  <autoFilter ref="B2:J60" xr:uid="{90B7AD45-2D83-4071-903A-709897297D7D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J60">
+    <sortCondition ref="B5:B60"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0D5FE4E1-CCB6-41E3-9CBA-4702C4DC05FF}" name="Code" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{82DC48B9-D439-409E-A599-04E67311C2CE}" name="Description" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{3349F41C-BA6E-4E46-9508-E2CE8AF2D286}" name="Purpose" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8C74FE47-B6E2-4502-B110-3924FBE0E4EA}" name="Project" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{E02829E7-E724-4627-909C-DDCAA29813CD}" name="Research File" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{8AFDD2DE-7025-4E27-A886-B2F06C5EAA27}" name="Acquisition file" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{CCB7DF0B-6A7E-4156-BF86-372D19F14DD9}" name="Lease/License" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{3B098A34-BB9A-4590-964F-6FBE2F24A1FF}" name="Disposition file" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{A7CAEE2F-B3DC-42CE-9683-0F8B0FF5ECFF}" name="Management" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1021,1462 +1462,1485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136C655F-10D5-4146-8405-A6BFCE94F80F}">
-  <dimension ref="B2:J59"/>
+  <dimension ref="B2:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.26953125" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="19.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="D5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="D10" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
+      <c r="D13" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="D14" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="4" t="s">
+      <c r="D16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D17" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B23" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B45" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B47" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J48" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B49" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B50" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B51" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" ht="58" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B52" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J52" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B53" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B55" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J55" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B56" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J56" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B57" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B58" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B59" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B60" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J60">
+    <sortCondition ref="B3:B60"/>
+  </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated sync helper to work with new format of files. Sorting before creating json to help in comparing. Other fixes (#4444)
Co-authored-by: Alejandro Sanchez <emailforasr@gmail.com>
</commit_message>
<xml_diff>
--- a/tools/mayan_sync_helper/xml_definitions/doctype_definitions.xlsx
+++ b/tools/mayan_sync_helper/xml_definitions/doctype_definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\pims\PSP\tools\mayan_sync_helper\xml_definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141F3229-BEBC-4E92-8A7B-606714F367F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D69F2FF-584D-4B3D-9DB4-77D2E8D16463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22320" yWindow="240" windowWidth="22185" windowHeight="20505" xr2:uid="{B36D4D41-52C3-4254-819B-044EB561F7B6}"/>
+    <workbookView xWindow="-38265" yWindow="0" windowWidth="18750" windowHeight="20985" xr2:uid="{B36D4D41-52C3-4254-819B-044EB561F7B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="195">
   <si>
     <t>Document type</t>
   </si>
@@ -427,175 +427,202 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>testing purpose 1</t>
-  </si>
-  <si>
-    <t>testing purpose 2</t>
-  </si>
-  <si>
-    <t>testing purpose 3</t>
-  </si>
-  <si>
-    <t>testing purpose 4</t>
-  </si>
-  <si>
-    <t>testing purpose 5</t>
-  </si>
-  <si>
-    <t>testing purpose 6</t>
-  </si>
-  <si>
-    <t>testing purpose 7</t>
-  </si>
-  <si>
-    <t>testing purpose 8</t>
-  </si>
-  <si>
-    <t>testing purpose 9</t>
-  </si>
-  <si>
-    <t>testing purpose 10</t>
-  </si>
-  <si>
-    <t>testing purpose 11</t>
-  </si>
-  <si>
-    <t>testing purpose 12</t>
-  </si>
-  <si>
-    <t>testing purpose 13</t>
-  </si>
-  <si>
-    <t>testing purpose 14</t>
-  </si>
-  <si>
-    <t>testing purpose 15</t>
-  </si>
-  <si>
-    <t>testing purpose 16</t>
-  </si>
-  <si>
-    <t>testing purpose 17</t>
-  </si>
-  <si>
-    <t>testing purpose 18</t>
-  </si>
-  <si>
-    <t>testing purpose 19</t>
-  </si>
-  <si>
-    <t>testing purpose 20</t>
-  </si>
-  <si>
-    <t>testing purpose 21</t>
-  </si>
-  <si>
-    <t>testing purpose 22</t>
-  </si>
-  <si>
-    <t>testing purpose 23</t>
-  </si>
-  <si>
-    <t>testing purpose 24</t>
-  </si>
-  <si>
-    <t>testing purpose 25</t>
-  </si>
-  <si>
-    <t>testing purpose 26</t>
-  </si>
-  <si>
-    <t>testing purpose 27</t>
-  </si>
-  <si>
-    <t>testing purpose 28</t>
-  </si>
-  <si>
-    <t>testing purpose 29</t>
-  </si>
-  <si>
-    <t>testing purpose 30</t>
-  </si>
-  <si>
-    <t>testing purpose 31</t>
-  </si>
-  <si>
-    <t>testing purpose 32</t>
-  </si>
-  <si>
-    <t>testing purpose 33</t>
-  </si>
-  <si>
-    <t>testing purpose 34</t>
-  </si>
-  <si>
-    <t>testing purpose 35</t>
-  </si>
-  <si>
-    <t>testing purpose 36</t>
-  </si>
-  <si>
-    <t>testing purpose 37</t>
-  </si>
-  <si>
-    <t>testing purpose 38</t>
-  </si>
-  <si>
-    <t>testing purpose 39</t>
-  </si>
-  <si>
-    <t>testing purpose 40</t>
-  </si>
-  <si>
-    <t>testing purpose 41</t>
-  </si>
-  <si>
-    <t>testing purpose 42</t>
-  </si>
-  <si>
-    <t>testing purpose 43</t>
-  </si>
-  <si>
-    <t>testing purpose 44</t>
-  </si>
-  <si>
-    <t>testing purpose 45</t>
-  </si>
-  <si>
-    <t>testing purpose 46</t>
-  </si>
-  <si>
-    <t>testing purpose 47</t>
-  </si>
-  <si>
-    <t>testing purpose 48</t>
-  </si>
-  <si>
-    <t>testing purpose 49</t>
-  </si>
-  <si>
-    <t>testing purpose 50</t>
-  </si>
-  <si>
-    <t>testing purpose 51</t>
-  </si>
-  <si>
-    <t>testing purpose 52</t>
-  </si>
-  <si>
-    <t>testing purpose 53</t>
-  </si>
-  <si>
-    <t>testing purpose 54</t>
-  </si>
-  <si>
-    <t>testing purpose 55</t>
-  </si>
-  <si>
-    <t>testing purpose 56</t>
-  </si>
-  <si>
-    <t>testing purpose 57</t>
+    <t xml:space="preserve">The Affidavit of Services and correspondence with the Process Server </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For ALC Applications, Orders, and Resolutions </t>
+  </si>
+  <si>
+    <t>Form 5 - Approval of expropriation</t>
+  </si>
+  <si>
+    <t>The Approval of Expropriation (Form 5) for Expropriations</t>
+  </si>
+  <si>
+    <t>Appraisals property in draft / final state</t>
+  </si>
+  <si>
+    <t>BC Assessment search</t>
+  </si>
+  <si>
+    <t>Draft / final versions of the briefing notes</t>
+  </si>
+  <si>
+    <t>Surveys registered in the Canada Land System.</t>
+  </si>
+  <si>
+    <t>Templates used for document generation in PIMS</t>
+  </si>
+  <si>
+    <t>The Certificate of Compliance (CoC)</t>
+  </si>
+  <si>
+    <t>The Certificate of Insurance H.0111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The compensation cheque </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The H.120 Compensation Requisitions </t>
+  </si>
+  <si>
+    <t>The company search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H.0443 Conditions of Entry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The conveyance closing documents which might include PTT, Form A Transfer, or Statement of Adjustments. </t>
+  </si>
+  <si>
+    <t>Attach letters, memos, emails (not record of negotiation, or legal correspondence)</t>
+  </si>
+  <si>
+    <t>The crown grant application and final crown grant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The District road register </t>
+  </si>
+  <si>
+    <t>The Referral Record for both incoming and outgoing referrals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The survey field notes </t>
+  </si>
+  <si>
+    <t>Financial records (invoices, journal vouchers, received cheques etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial records which could include invoices, JV’s, contracts ect. </t>
+  </si>
+  <si>
+    <t>Record of engagement with first nations (ex: First Nations Consultation Log)</t>
+  </si>
+  <si>
+    <t>The First Nation Strength of Claim report</t>
+  </si>
+  <si>
+    <t>Form 12 - Certificate As To Highway In Statutory Right Of Way Plan, pre and post registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gazette notices – all types of gazettes (establishing, closing, widening, erratum’s) </t>
+  </si>
+  <si>
+    <t>All types of scanned documents from a historical file</t>
+  </si>
+  <si>
+    <t>Applications and final Land Act Tenure Reserves (Sections 15/16/17)</t>
+  </si>
+  <si>
+    <t>Lease / License agreement</t>
+  </si>
+  <si>
+    <t>Draft or Final Lease/License agreement, amending agreement or extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emails or letters with internal and external lawyers </t>
+  </si>
+  <si>
+    <t>Attach copies of legal survey plans, draft or registered versions</t>
+  </si>
+  <si>
+    <t>Approval/sign-off</t>
+  </si>
+  <si>
+    <t>The record of correspondence (email) approving Lease/Licence</t>
+  </si>
+  <si>
+    <t>Attach LTSA documents ie: copies of mortgages, SRW’s, Easements, Pending Litigation (except title searches and legal plans)</t>
+  </si>
+  <si>
+    <t>Ministerial Orders</t>
+  </si>
+  <si>
+    <t>Miscellaneous Notes from the property title</t>
+  </si>
+  <si>
+    <t>Moti Plans, plans not found in LTSA (Road Surveys)</t>
+  </si>
+  <si>
+    <t>NOTIABANDON</t>
+  </si>
+  <si>
+    <t>Form 7 - Notice of abandonement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form 8 - Notice of advanced payment </t>
+  </si>
+  <si>
+    <t>The Notice of Advance Payment  (Form 8) for Expropriation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Notice of Claims/Litigation documents </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form 1 - Notice of expropriation </t>
+  </si>
+  <si>
+    <t>The Notice of Expropriation (Form 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Notice of Possible Entry (H.0224) </t>
+  </si>
+  <si>
+    <t>The Order in Council</t>
+  </si>
+  <si>
+    <t>Uncategorized / Miscellaneous document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other forms of Land Agreements such as Indemnity Letters, Letter of Intended Use, Assumption Agreements etc. </t>
+  </si>
+  <si>
+    <t>Attach copies of draft or final Offer to Purchase agreements (H.179s) or external Owner agreements for Offer and Purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property acquisition drawings, design drawings, engineered drawings in draft and final versions </t>
+  </si>
+  <si>
+    <t>Attach Photos, images or videos relevant to file/property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Privy Council </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional/Expert Report in draft or final (Ie: Geotechnical, Environmental, Archeology, Engineering Reports)  </t>
+  </si>
+  <si>
+    <t>The Purchase and Sale Agreement for a road closure file (H.179RC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Record of Negotiations </t>
+  </si>
+  <si>
+    <t>The Release of Claims document, Draft and Final versions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Spending Authority Approval (SAA) document, Draft and Final versions </t>
+  </si>
+  <si>
+    <t>The Surplus Property Declarations document in Draft or Final indicating surplus land</t>
+  </si>
+  <si>
+    <t>Tax notices or Tax assessments</t>
+  </si>
+  <si>
+    <t>The Temporary License for Construction Access Agreement (TLCA) Draft or Final version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Title Search from LTSA which could be a current or historical search </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Transfer of Administration (TAC) document – Draft or Final version </t>
+  </si>
+  <si>
+    <t>Form 9 - Vesting notice (Form 9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Vesting Notice (Form 9) for Expropriations </t>
   </si>
 </sst>
 </file>
@@ -604,14 +631,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -638,9 +657,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FFB6C2CF"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -664,7 +690,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -687,31 +713,425 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -722,6 +1142,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90B7AD45-2D83-4071-903A-709897297D7D}" name="Table1" displayName="Table1" ref="B2:J60" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="11" totalsRowBorderDxfId="10" headerRowCellStyle="Normal">
+  <autoFilter ref="B2:J60" xr:uid="{90B7AD45-2D83-4071-903A-709897297D7D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J60">
+    <sortCondition ref="B5:B60"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0D5FE4E1-CCB6-41E3-9CBA-4702C4DC05FF}" name="Code" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{82DC48B9-D439-409E-A599-04E67311C2CE}" name="Description" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{3349F41C-BA6E-4E46-9508-E2CE8AF2D286}" name="Purpose" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8C74FE47-B6E2-4502-B110-3924FBE0E4EA}" name="Project" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{E02829E7-E724-4627-909C-DDCAA29813CD}" name="Research File" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{8AFDD2DE-7025-4E27-A886-B2F06C5EAA27}" name="Acquisition file" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{CCB7DF0B-6A7E-4156-BF86-372D19F14DD9}" name="Lease/License" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{3B098A34-BB9A-4590-964F-6FBE2F24A1FF}" name="Disposition file" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{A7CAEE2F-B3DC-42CE-9683-0F8B0FF5ECFF}" name="Management" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1021,1462 +1462,1485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136C655F-10D5-4146-8405-A6BFCE94F80F}">
-  <dimension ref="B2:J59"/>
+  <dimension ref="B2:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.26953125" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="19.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="D5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="D10" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
+      <c r="D13" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="D14" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="4" t="s">
+      <c r="D16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D17" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B23" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B45" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B47" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J48" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B49" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B50" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B51" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" ht="58" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B52" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J52" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B53" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B55" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J55" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B56" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J56" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B57" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B58" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B59" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B60" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J60">
+    <sortCondition ref="B3:B60"/>
+  </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated document types (#4592)
</commit_message>
<xml_diff>
--- a/tools/mayan_sync_helper/xml_definitions/doctype_definitions.xlsx
+++ b/tools/mayan_sync_helper/xml_definitions/doctype_definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\pims\PSP\tools\mayan_sync_helper\xml_definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D69F2FF-584D-4B3D-9DB4-77D2E8D16463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BACCDBB-D2B5-46B1-B657-4BB0052146B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38265" yWindow="0" windowWidth="18750" windowHeight="20985" xr2:uid="{B36D4D41-52C3-4254-819B-044EB561F7B6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B36D4D41-52C3-4254-819B-044EB561F7B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="195">
   <si>
     <t>Document type</t>
   </si>
@@ -427,12 +427,6 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t xml:space="preserve">The Affidavit of Services and correspondence with the Process Server </t>
-  </si>
-  <si>
-    <t xml:space="preserve">For ALC Applications, Orders, and Resolutions </t>
-  </si>
-  <si>
     <t>Form 5 - Approval of expropriation</t>
   </si>
   <si>
@@ -448,9 +442,6 @@
     <t>Draft / final versions of the briefing notes</t>
   </si>
   <si>
-    <t>Surveys registered in the Canada Land System.</t>
-  </si>
-  <si>
     <t>Templates used for document generation in PIMS</t>
   </si>
   <si>
@@ -460,42 +451,18 @@
     <t>The Certificate of Insurance H.0111</t>
   </si>
   <si>
-    <t xml:space="preserve">The compensation cheque </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The H.120 Compensation Requisitions </t>
-  </si>
-  <si>
     <t>The company search</t>
   </si>
   <si>
-    <t xml:space="preserve">H.0443 Conditions of Entry </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The conveyance closing documents which might include PTT, Form A Transfer, or Statement of Adjustments. </t>
-  </si>
-  <si>
     <t>Attach letters, memos, emails (not record of negotiation, or legal correspondence)</t>
   </si>
   <si>
     <t>The crown grant application and final crown grant</t>
   </si>
   <si>
-    <t xml:space="preserve">The District road register </t>
-  </si>
-  <si>
-    <t>The Referral Record for both incoming and outgoing referrals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The survey field notes </t>
-  </si>
-  <si>
     <t>Financial records (invoices, journal vouchers, received cheques etc.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial records which could include invoices, JV’s, contracts ect. </t>
-  </si>
-  <si>
     <t>Record of engagement with first nations (ex: First Nations Consultation Log)</t>
   </si>
   <si>
@@ -505,9 +472,6 @@
     <t>Form 12 - Certificate As To Highway In Statutory Right Of Way Plan, pre and post registration</t>
   </si>
   <si>
-    <t xml:space="preserve">Gazette notices – all types of gazettes (establishing, closing, widening, erratum’s) </t>
-  </si>
-  <si>
     <t>All types of scanned documents from a historical file</t>
   </si>
   <si>
@@ -520,9 +484,6 @@
     <t>Draft or Final Lease/License agreement, amending agreement or extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Emails or letters with internal and external lawyers </t>
-  </si>
-  <si>
     <t>Attach copies of legal survey plans, draft or registered versions</t>
   </si>
   <si>
@@ -556,54 +517,30 @@
     <t>The Notice of Advance Payment  (Form 8) for Expropriation</t>
   </si>
   <si>
-    <t xml:space="preserve">The Notice of Claims/Litigation documents </t>
-  </si>
-  <si>
     <t xml:space="preserve">Form 1 - Notice of expropriation </t>
   </si>
   <si>
     <t>The Notice of Expropriation (Form 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">The Notice of Possible Entry (H.0224) </t>
-  </si>
-  <si>
     <t>The Order in Council</t>
   </si>
   <si>
     <t>Uncategorized / Miscellaneous document</t>
   </si>
   <si>
-    <t xml:space="preserve">Other forms of Land Agreements such as Indemnity Letters, Letter of Intended Use, Assumption Agreements etc. </t>
-  </si>
-  <si>
     <t>Attach copies of draft or final Offer to Purchase agreements (H.179s) or external Owner agreements for Offer and Purchase</t>
   </si>
   <si>
-    <t xml:space="preserve">Property acquisition drawings, design drawings, engineered drawings in draft and final versions </t>
-  </si>
-  <si>
     <t>Attach Photos, images or videos relevant to file/property</t>
   </si>
   <si>
-    <t xml:space="preserve">The Privy Council </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professional/Expert Report in draft or final (Ie: Geotechnical, Environmental, Archeology, Engineering Reports)  </t>
-  </si>
-  <si>
     <t>The Purchase and Sale Agreement for a road closure file (H.179RC)</t>
   </si>
   <si>
-    <t xml:space="preserve">The Record of Negotiations </t>
-  </si>
-  <si>
     <t>The Release of Claims document, Draft and Final versions</t>
   </si>
   <si>
-    <t xml:space="preserve">The Spending Authority Approval (SAA) document, Draft and Final versions </t>
-  </si>
-  <si>
     <t>The Surplus Property Declarations document in Draft or Final indicating surplus land</t>
   </si>
   <si>
@@ -613,16 +550,79 @@
     <t>The Temporary License for Construction Access Agreement (TLCA) Draft or Final version</t>
   </si>
   <si>
-    <t xml:space="preserve">The Title Search from LTSA which could be a current or historical search </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Transfer of Administration (TAC) document – Draft or Final version </t>
-  </si>
-  <si>
     <t>Form 9 - Vesting notice (Form 9)</t>
   </si>
   <si>
-    <t xml:space="preserve">The Vesting Notice (Form 9) for Expropriations </t>
+    <t>The Affidavit of Services and correspondence with the Process Server</t>
+  </si>
+  <si>
+    <t>For ALC Applications, Orders, and Resolutions</t>
+  </si>
+  <si>
+    <t>Surveys registered in the Canada Land System</t>
+  </si>
+  <si>
+    <t>The compensation cheque</t>
+  </si>
+  <si>
+    <t>The H.120 Compensation Requisitions</t>
+  </si>
+  <si>
+    <t>H.0443 Conditions of Entry</t>
+  </si>
+  <si>
+    <t>The conveyance closing documents which might include PTT, Form A Transfer, or Statement of Adjustments</t>
+  </si>
+  <si>
+    <t>The District road register</t>
+  </si>
+  <si>
+    <t>The Referral Record for both incoming and outgoing referrals</t>
+  </si>
+  <si>
+    <t>The survey field notes</t>
+  </si>
+  <si>
+    <t>Gazette notices – all types of gazettes (establishing, closing, widening, erratum’s)</t>
+  </si>
+  <si>
+    <t>Emails or letters with internal and external lawyers</t>
+  </si>
+  <si>
+    <t>The Notice of Claims/Litigation documents</t>
+  </si>
+  <si>
+    <t>The Notice of Possible Entry (H.0224)</t>
+  </si>
+  <si>
+    <t>Other forms of Land Agreements such as Indemnity Letters, Letter of Intended Use, Assumption Agreements etc.</t>
+  </si>
+  <si>
+    <t>Property acquisition drawings, design drawings, engineered drawings in draft and final versions</t>
+  </si>
+  <si>
+    <t>The Privy Council</t>
+  </si>
+  <si>
+    <t>Professional/Expert Report in draft or final (Ie: Geotechnical, Environmental, Archeology, Engineering Reports)</t>
+  </si>
+  <si>
+    <t>The Record of Negotiations</t>
+  </si>
+  <si>
+    <t>The Spending Authority Approval (SAA) document, Draft and Final versions</t>
+  </si>
+  <si>
+    <t>The Title Search from LTSA which could be a current or historical search</t>
+  </si>
+  <si>
+    <t>The Transfer of Administration (TAC) document – Draft or Final version</t>
+  </si>
+  <si>
+    <t>The Vesting Notice (Form 9) for Expropriations</t>
+  </si>
+  <si>
+    <t>Financial records which could include invoices, JV’s, contracts etc.</t>
   </si>
 </sst>
 </file>
@@ -783,25 +783,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1131,6 +1112,25 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1145,21 +1145,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90B7AD45-2D83-4071-903A-709897297D7D}" name="Table1" displayName="Table1" ref="B2:J60" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="11" totalsRowBorderDxfId="10" headerRowCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90B7AD45-2D83-4071-903A-709897297D7D}" name="Table1" displayName="Table1" ref="B2:J60" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9" headerRowCellStyle="Normal">
   <autoFilter ref="B2:J60" xr:uid="{90B7AD45-2D83-4071-903A-709897297D7D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J60">
     <sortCondition ref="B5:B60"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0D5FE4E1-CCB6-41E3-9CBA-4702C4DC05FF}" name="Code" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{82DC48B9-D439-409E-A599-04E67311C2CE}" name="Description" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{3349F41C-BA6E-4E46-9508-E2CE8AF2D286}" name="Purpose" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8C74FE47-B6E2-4502-B110-3924FBE0E4EA}" name="Project" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{E02829E7-E724-4627-909C-DDCAA29813CD}" name="Research File" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{8AFDD2DE-7025-4E27-A886-B2F06C5EAA27}" name="Acquisition file" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{CCB7DF0B-6A7E-4156-BF86-372D19F14DD9}" name="Lease/License" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{3B098A34-BB9A-4590-964F-6FBE2F24A1FF}" name="Disposition file" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{A7CAEE2F-B3DC-42CE-9683-0F8B0FF5ECFF}" name="Management" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{0D5FE4E1-CCB6-41E3-9CBA-4702C4DC05FF}" name="Code" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{82DC48B9-D439-409E-A599-04E67311C2CE}" name="Description" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3349F41C-BA6E-4E46-9508-E2CE8AF2D286}" name="Purpose" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{8C74FE47-B6E2-4502-B110-3924FBE0E4EA}" name="Project" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{E02829E7-E724-4627-909C-DDCAA29813CD}" name="Research File" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{8AFDD2DE-7025-4E27-A886-B2F06C5EAA27}" name="Acquisition file" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{CCB7DF0B-6A7E-4156-BF86-372D19F14DD9}" name="Lease/License" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{3B098A34-BB9A-4590-964F-6FBE2F24A1FF}" name="Disposition file" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{A7CAEE2F-B3DC-42CE-9683-0F8B0FF5ECFF}" name="Management" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1464,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136C655F-10D5-4146-8405-A6BFCE94F80F}">
   <dimension ref="B2:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1519,7 +1519,7 @@
         <v>41</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1540,7 +1540,7 @@
         <v>123</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1556,10 +1556,10 @@
         <v>91</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -1580,7 +1580,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1605,7 +1605,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
@@ -1632,7 +1632,7 @@
         <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>7</v>
@@ -1661,7 +1661,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
@@ -1686,7 +1686,7 @@
         <v>107</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1705,7 +1705,7 @@
         <v>115</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1726,7 +1726,7 @@
         <v>46</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -1751,7 +1751,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -1774,7 +1774,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1797,7 +1797,7 @@
         <v>27</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
@@ -1824,7 +1824,7 @@
         <v>35</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
@@ -1847,11 +1847,13 @@
         <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="H17" s="7" t="s">
         <v>7</v>
       </c>
@@ -1870,7 +1872,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>7</v>
@@ -1899,7 +1901,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="s">
@@ -1922,7 +1924,7 @@
         <v>20</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
@@ -1947,7 +1949,7 @@
         <v>114</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1968,7 +1970,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
@@ -1990,10 +1992,10 @@
         <v>108</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>7</v>
@@ -2022,7 +2024,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
@@ -2049,7 +2051,7 @@
         <v>116</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -2070,7 +2072,7 @@
         <v>125</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
@@ -2097,7 +2099,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
@@ -2124,7 +2126,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>7</v>
@@ -2153,7 +2155,7 @@
         <v>127</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2169,10 +2171,10 @@
         <v>57</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7" t="s">
@@ -2197,7 +2199,7 @@
         <v>52</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>7</v>
@@ -2226,7 +2228,7 @@
         <v>16</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>7</v>
@@ -2252,10 +2254,10 @@
         <v>99</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2276,7 +2278,7 @@
         <v>28</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7" t="s">
@@ -2303,7 +2305,7 @@
         <v>15</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
@@ -2328,7 +2330,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7" t="s">
@@ -2355,7 +2357,7 @@
         <v>13</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>7</v>
@@ -2378,10 +2380,10 @@
     </row>
     <row r="38" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="4" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
@@ -2398,10 +2400,10 @@
         <v>88</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -2422,7 +2424,7 @@
         <v>45</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7" t="s">
@@ -2444,10 +2446,10 @@
         <v>90</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2468,7 +2470,7 @@
         <v>42</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7" t="s">
@@ -2491,7 +2493,7 @@
         <v>12</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7" t="s">
@@ -2516,7 +2518,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>7</v>
@@ -2545,7 +2547,7 @@
         <v>54</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -2570,7 +2572,7 @@
         <v>84</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7" t="s">
@@ -2593,7 +2595,7 @@
         <v>10</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>7</v>
@@ -2618,7 +2620,7 @@
         <v>69</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>7</v>
@@ -2647,7 +2649,7 @@
         <v>8</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7" t="s">
@@ -2670,7 +2672,7 @@
         <v>30</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E50" s="7"/>
       <c r="F50" s="7" t="s">
@@ -2697,7 +2699,7 @@
         <v>113</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -2718,7 +2720,7 @@
         <v>53</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
@@ -2741,7 +2743,7 @@
         <v>37</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
@@ -2764,7 +2766,7 @@
         <v>82</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>7</v>
@@ -2791,7 +2793,7 @@
         <v>49</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>7</v>
@@ -2818,7 +2820,7 @@
         <v>44</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7" t="s">
@@ -2845,7 +2847,7 @@
         <v>50</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -2915,10 +2917,10 @@
         <v>92</v>
       </c>
       <c r="C60" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>194</v>
       </c>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>

</xml_diff>